<commit_message>
fix incidencias CI 1-5
</commit_message>
<xml_diff>
--- a/desarrollo/rigk-sg-back/files/templates/_carga_masiva_1.xlsx
+++ b/desarrollo/rigk-sg-back/files/templates/_carga_masiva_1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>TIPO TRATAMIENTO</t>
   </si>
@@ -41,16 +41,16 @@
     <t>PapelCartón</t>
   </si>
   <si>
-    <t>Cartón: cajas</t>
-  </si>
-  <si>
-    <t>Aluminio: latas, rejas IBC</t>
-  </si>
-  <si>
-    <t>Rígido: bidones, tambores, botellas, IBC, tinetas</t>
-  </si>
-  <si>
-    <t>Pallet</t>
+    <t>Papel</t>
+  </si>
+  <si>
+    <t>Envase Aluminio</t>
+  </si>
+  <si>
+    <t>Plástico Film Embalaje</t>
+  </si>
+  <si>
+    <t>Caja de Madera</t>
   </si>
   <si>
     <t>2 - Quinta Región - Los Aromos 2432</t>
@@ -59,16 +59,16 @@
     <t>Valorización Energética</t>
   </si>
   <si>
-    <t>Cartón: esquineros, conos</t>
-  </si>
-  <si>
-    <t>Fierro: hojalata, tambores, zunchos, tinetas, tanques</t>
-  </si>
-  <si>
-    <t>Rígido: pallets, bins</t>
-  </si>
-  <si>
-    <t>Cajas, esquineros, carretes</t>
+    <t>Papel Compuesto (cemento)</t>
+  </si>
+  <si>
+    <t>Malla o Reja (IBC)</t>
+  </si>
+  <si>
+    <t>Plástico Envases Rígidos (Incl. Tapas)</t>
+  </si>
+  <si>
+    <t>Pallet de Madera</t>
   </si>
   <si>
     <t>5 - Región de Los Lagos - Establecimiento</t>
@@ -77,39 +77,42 @@
     <t>Disposición Final en RS</t>
   </si>
   <si>
-    <t>Papel: bolsas, papel kraft, manuales</t>
-  </si>
-  <si>
-    <t>Flexibles rafia: sacos, maxisacos</t>
+    <t>Caja Cartón</t>
+  </si>
+  <si>
+    <t>Envase Hojalata</t>
+  </si>
+  <si>
+    <t>Plástico Sacos o Maxisacos</t>
   </si>
   <si>
     <t>73 - Región de O’Higgins - Ejemplo</t>
   </si>
   <si>
-    <t>Papel compuesto: bolsas de cemento, linear</t>
-  </si>
-  <si>
-    <t>Flexibles láminas: films de embalaje, bolsas, burbujas, contraible, flexitank</t>
+    <t>Papel/Cartón Otro</t>
+  </si>
+  <si>
+    <t>Metal Otro</t>
+  </si>
+  <si>
+    <t>Plástico EPS (Poliestireno Expandido)</t>
   </si>
   <si>
     <t>104 - Región de Coquimbo - Nombre</t>
   </si>
   <si>
-    <t>Flexibles: zunchos</t>
+    <t>Plástico Zuncho</t>
   </si>
   <si>
     <t>125 - Región de Atacama - Juan</t>
   </si>
   <si>
-    <t>Poliestireno: cajas, protecciones, bandejas</t>
+    <t>Plástico Otro</t>
   </si>
   <si>
     <t>156 - Región de Antofagasta - juan</t>
   </si>
   <si>
-    <t>Plásticos compuestos: multicapas</t>
-  </si>
-  <si>
     <t>157 - Región de Arica y Parinacota - Juan</t>
   </si>
   <si>
@@ -146,7 +149,7 @@
     <t>NOMBRE GESTOR</t>
   </si>
   <si>
-    <t>RUT ESTABLECIMIENTO RECEPTOR</t>
+    <t>RUT GESTOR</t>
   </si>
   <si>
     <t>CÓDIGO ESTABLECIMIENTO RECEPTOR</t>
@@ -191,8 +194,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -235,8 +239,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" name="Metal" displayName="Metal" ref="E1:E3" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="E1:E3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" name="Metal" displayName="Metal" ref="E1:E5" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="E1:E5">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
@@ -247,8 +251,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" name="Plástico" displayName="Plástico" ref="F1:F8" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="F1:F8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" name="Plástico" displayName="Plástico" ref="F1:F7" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="F1:F7">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
@@ -680,71 +684,74 @@
       <c r="D4" t="s">
         <v>21</v>
       </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -773,92 +780,192 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="58">
     <dataValidation type="list" showErrorMessage="1" error="aaaa" sqref="A10:A51">
@@ -867,11 +974,13 @@
     <dataValidation type="list" showErrorMessage="1" error="aaaa" sqref="A2:A51">
       <formula1>Info!$A$2:$A$13</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="lessThanOrEqual" showErrorMessage="1" errorStyle="error" errorTitle="Fecha Inválida" error="No debe superar la fecha de hoy" sqref="B10:B51">
-      <formula1>45042.8485097338</formula1>
-    </dataValidation>
-    <dataValidation type="date" operator="lessThanOrEqual" showErrorMessage="1" errorStyle="error" errorTitle="Fecha Inválida" error="No debe superar la fecha de hoy" sqref="B2:B51">
-      <formula1>45042.8485097338</formula1>
+    <dataValidation type="textLength" showErrorMessage="1" errorStyle="error" errorTitle="Formato de Fecha Inválido" error="Por favor, ingrese una fecha válida en formato DD/MM/AAAA." sqref="B10:B51">
+      <formula1>10</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" showErrorMessage="1" errorStyle="error" errorTitle="Formato de Fecha Inválido" error="Por favor, ingrese una fecha válida en formato DD/MM/AAAA." sqref="B2:B51">
+      <formula1>10</formula1>
+      <formula2>10</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="D10:D51">
       <formula1>Info!$B$2:$B$4</formula1>

</xml_diff>